<commit_message>
Commit de mudanças no tesseract
</commit_message>
<xml_diff>
--- a/rubricas.xlsx
+++ b/rubricas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B28"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,324 +448,84 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>7</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2HORAS NOTURNAS [+] Provento Horas Nenhuma Salários i] Não Não ES Não Não Sim</t>
+          <t>HORAS JUSTIFICADAS 7 Provento Horas Nenhuma Horas Justificadas 0 Não Não Não Não Não Sim</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1213</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>3HORAS FERIAS 7 Provento Horas Nerhuma Férias Gozadas 0 Não Não Não Não Não Sim</t>
+          <t>SALARIO INTEGRAL 79 Provento Valor Nenhuma 13º Salário 0 Não Não Não Não Não Sim</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1313</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>4SALÁRIO MATERNIDADE n Provento Horas Nenhuma Salários 0 Não Não Não E E Sim</t>
+          <t>SALARIO ADIANTADO 80 Provento Valor Nenhuma 13! Salário 0 Não Não Não Não Não Sim</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>22</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>5SHORAS AFAST.INSS (P/DOENC 72 Provento Horas Nenhuma Salários 0 E E Não E) E) Sim</t>
+          <t>AVISO PREVIO 8 Provento Valor Nenhuma Aviso Prévio 0 Não Não Não Não Não Sim</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>26</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>7 HORAS JUSTIFICADAS 7 Provento Horas Nerhuma Horas Justificadas 0 Não Não Não Não Não Sim</t>
+          <t>ADICIONAL NOTURNO (AUTOM) 89 Provento Horas Salário Contratual Adicional Noturno 20,0000 Sim Sim Sim Não Não Sim</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>37</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>BHORAS AFAST S/VENCTO 7 Provento Horas Nenhuma Salários 0 Não Não Não E E Sim</t>
+          <t>COMISSOES s2 Provento Valor Nenhuma Comissão 0 Sim Sim Sim Não Não Sim</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>41</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>TOHORAS REPOUSO REMUNERADO EA Provento Horas Nenhuma Salários i] Não Não Não Não Não Sim</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>1213 SALARIO INTEGRAL 79 Provento Valor Nenhuma 13º Salário 0 Não Não Não E E Sim</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>1313 SALARIO ADIANTADO 8 Provento Valor Nenhuma 13º Salário 0 E E Não E) E) Sim</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>15INSALUBRIDADE 10% a Provento Automático Salário Mínimo Insalubridade 10,0000 Não Não Não Sim Sim Sim</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>16INSALUBRIDADE 20% EA Provento Automático Salário Mínimo Insalubridade 20,0000 Não Não Não Sim Sim Sim</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>17</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>17INSALUBRIDADE 40% 8 Provento Automático Salário Mínimo Insalubridade 40,0000 Não Não Não Sim Sim Sim</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>18AUXILIO NATALIDADE 8 Provento Valor Salário Mínimo Dutros Proventos 0 E E Não E) E) Sim</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>19</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>19DIFERENCA DE SALARIOS 8 Provento Valor Nenhuma Dutros Proventos i] Não Não Não Não Não Sim</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>20GRATIFICACOES 86 Provento Valor Nerhuma Gratificação 0 Sim Sim Sim Não Não Sim</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>22 AVISO PREVIO EIA Provento Valor Nenhuma Aviso Prévio 0 Não Não Não E E Sim</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>23F.G.7.5 DE RESCISAO VIZs Informativa Valor Nenhuma FGTS -GRRF 8,0000 E E Não E) E) Sim</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>24F.G.7.S MES ANTERIOR 1077 Informativa Valor Nenhuma FGTS -GRRF i] Não Não Não Não Não Sim</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>25ADICIONAL NOTURNO (INFOR) 88 Provento Horas Salário Contratual Adicional Notumo 20,0000 Sim Sim Sim Não Não Sim</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>26</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>26 ADICIONAL NOTURNO (AUTOM) 89 Provento Horas Salário Contratual Adicional Noturno 20,0000 Sim Sim Sim E E Sim</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>28</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>28FERIAS VENCIDAS so Provento Valor Nenhuma Férias Rescisão 0 E E Não E) E) Sim</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>28</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>29FERIAS PROPORCIONAIS gs Provento Valor Nenhuma Férias Rescisão i] Não Não Não Não Não Sim</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>32</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>QF.GT.s 40% 1176 Informativa Valor Nerhuma FGTS -GRRF 40,0000 Não Não Não Não Não Sim</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>35</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>35FGTS 130 SALARIO RESCISAO 1162 Informativa Valor Nenhuma FGTS -GRRF 8,0000 E E Não E) E) Sim</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>40</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>40HORAS FALTAS 93 Desconto Horas Salário Contratual Falta Integral 0 Não Não Não Não Não Sim</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>41 HORAS INATIVAS E Desconto Horas Nenhuma Descontos 0 Não Não Não E E Sim</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>42</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>42HORAS FALTAS DSR s Desconto Horas Salário Contratual Descontos 0 DE DE Não Não E) Sim</t>
+          <t>HORAS INATIVAS Eu Desconto Horas Nenhuma Descontos 0 Não Não Não Não Não Sim</t>
         </is>
       </c>
     </row>

</xml_diff>